<commit_message>
PFC2 - Lucas [0.5]
Código depois da reunião do dia 25/06. Antes do desenvolvimento da classe "Kahoot Report"
</commit_message>
<xml_diff>
--- a/ParserXLS/kahoot_12_09_2018.xlsx
+++ b/ParserXLS/kahoot_12_09_2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12375" tabRatio="500" activeTab="7"/>
+    <workbookView windowWidth="28800" windowHeight="12510" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -370,16 +370,16 @@
   <numFmts count="12">
     <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="0.00%&quot; No&quot;"/>
-    <numFmt numFmtId="179" formatCode="0.00&quot; points&quot;"/>
+    <numFmt numFmtId="178" formatCode="0.00%&quot; Yes&quot;"/>
+    <numFmt numFmtId="179" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="180" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="181" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="182" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="183" formatCode="0.00&quot; out of 5&quot;"/>
-    <numFmt numFmtId="184" formatCode="0.00%&quot; Yes&quot;"/>
-    <numFmt numFmtId="185" formatCode="0.00%&quot; Positive&quot;"/>
-    <numFmt numFmtId="186" formatCode="0.00%&quot; Negative&quot;"/>
-    <numFmt numFmtId="187" formatCode="0.00%&quot; Neutral&quot;"/>
+    <numFmt numFmtId="181" formatCode="0.00%&quot; Negative&quot;"/>
+    <numFmt numFmtId="182" formatCode="0.00&quot; points&quot;"/>
+    <numFmt numFmtId="183" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="184" formatCode="0.00%&quot; Positive&quot;"/>
+    <numFmt numFmtId="185" formatCode="0.00&quot; out of 5&quot;"/>
+    <numFmt numFmtId="186" formatCode="0.00%&quot; Neutral&quot;"/>
+    <numFmt numFmtId="187" formatCode="0.00%&quot; No&quot;"/>
   </numFmts>
   <fonts count="36">
     <font>
@@ -483,6 +483,11 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -492,17 +497,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -513,29 +510,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -565,44 +542,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -617,6 +556,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -625,8 +572,61 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -731,7 +731,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -743,13 +761,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -761,7 +815,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -773,31 +851,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -809,19 +863,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -839,13 +893,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -857,55 +905,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1100,45 +1100,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1184,6 +1145,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1197,140 +1173,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="177" fontId="20" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="20" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="20" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="183" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="20" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="43" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="31" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="17" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1476,40 +1476,40 @@
     <xf numFmtId="49" fontId="12" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="12" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="179" fontId="12" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="183" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="185" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="187" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="184" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="185" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="187" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="186" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="186" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1901,8 +1901,8 @@
   <sheetPr/>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" outlineLevelCol="7"/>
@@ -2209,7 +2209,7 @@
   <sheetPr/>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:B21"/>
     </sheetView>
   </sheetViews>
@@ -3576,7 +3576,7 @@
   <sheetPr/>
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="B15" sqref="B15:B32"/>
     </sheetView>
   </sheetViews>
@@ -7036,8 +7036,8 @@
   <sheetPr/>
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B32" sqref="B15:B32"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>

</xml_diff>